<commit_message>
correct sum-ref issue, update stats and figures
</commit_message>
<xml_diff>
--- a/data/WhyWomenKill.xlsx
+++ b/data/WhyWomenKill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dartmouth-my.sharepoint.com/personal/f00481t_dartmouth_edu/Documents/CDL/prediction-retrodiction-paper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{D9728D18-3D90-D84F-8A9A-D3C076B1F469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E443E87-FB35-E044-AFA7-96870D7EFA99}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{D9728D18-3D90-D84F-8A9A-D3C076B1F469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0F069DA-05CE-4242-B5CC-B8A873E54739}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37320" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14960" yWindow="500" windowWidth="48840" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info_for_pub" sheetId="46" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">references!$A$1:$N$90</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">references_addi!$A$1:$K$19</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="158">
   <si>
     <t>story</t>
   </si>
@@ -1123,6 +1123,15 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">They always wear the same dowdy clothes. They don't change their hair. </t>
+  </si>
+  <si>
+    <t>The worst. My best engineer quit today, my secretary called in sick, and on top of all that, I took my boss's briefcase home by mistake.</t>
+  </si>
+  <si>
+    <t>amended</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1235,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1269,7 +1278,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1282,6 +1290,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Good" xfId="5" builtinId="26"/>
@@ -1566,7 +1578,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -1991,11 +2003,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AT93"/>
+  <dimension ref="A1:AT95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -2010,7 +2022,8 @@
     <col min="10" max="10" width="6.36328125" style="7" customWidth="1"/>
     <col min="11" max="11" width="7.54296875" style="7" customWidth="1"/>
     <col min="12" max="12" width="97" style="14" customWidth="1"/>
-    <col min="14" max="46" width="10.6328125" style="3"/>
+    <col min="14" max="14" width="10.6328125" style="3"/>
+    <col min="16" max="46" width="10.6328125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="30" x14ac:dyDescent="0.35">
@@ -2056,6 +2069,9 @@
       <c r="N1" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="O1" s="25" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="2" spans="1:46" ht="30" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
@@ -2098,7 +2114,6 @@
       <c r="N2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
       <c r="R2"/>
@@ -2172,7 +2187,6 @@
       <c r="N3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O3"/>
       <c r="P3"/>
       <c r="Q3"/>
       <c r="R3"/>
@@ -2246,7 +2260,6 @@
       <c r="N4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4"/>
@@ -2320,7 +2333,6 @@
       <c r="N5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
       <c r="R5"/>
@@ -2512,7 +2524,7 @@
         <v>28</v>
       </c>
       <c r="K9" s="10"/>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="20" t="s">
         <v>148</v>
       </c>
       <c r="M9" s="10" t="s">
@@ -2521,6 +2533,7 @@
       <c r="N9" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="O9"/>
     </row>
     <row r="10" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
@@ -2555,7 +2568,7 @@
         <v>28</v>
       </c>
       <c r="K10" s="10"/>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="20" t="s">
         <v>149</v>
       </c>
       <c r="M10" s="10" t="s">
@@ -2564,6 +2577,7 @@
       <c r="N10" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="O10"/>
     </row>
     <row r="11" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
@@ -2591,7 +2605,7 @@
       <c r="H11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>27</v>
       </c>
       <c r="J11" s="10" t="s">
@@ -2607,6 +2621,7 @@
       <c r="N11" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="O11"/>
     </row>
     <row r="12" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
@@ -2634,7 +2649,7 @@
       <c r="H12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="21" t="s">
         <v>27</v>
       </c>
       <c r="J12" s="10" t="s">
@@ -2650,6 +2665,7 @@
       <c r="N12" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="O12"/>
     </row>
     <row r="13" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
@@ -2693,6 +2709,7 @@
       <c r="N13" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="O13"/>
     </row>
     <row r="14" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
@@ -2736,6 +2753,7 @@
       <c r="N14" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="O14"/>
     </row>
     <row r="15" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
@@ -2770,7 +2788,7 @@
         <v>28</v>
       </c>
       <c r="K15" s="10"/>
-      <c r="L15" s="21" t="s">
+      <c r="L15" s="20" t="s">
         <v>29</v>
       </c>
       <c r="M15" s="10" t="s">
@@ -2779,6 +2797,7 @@
       <c r="N15" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="O15"/>
     </row>
     <row r="16" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
@@ -2822,8 +2841,9 @@
       <c r="N16" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>1</v>
       </c>
@@ -2865,8 +2885,9 @@
       <c r="N17" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="1:15" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>1</v>
       </c>
@@ -2883,7 +2904,7 @@
       <c r="E18" s="10">
         <v>403</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="23">
         <v>303</v>
       </c>
       <c r="G18" s="10">
@@ -2908,8 +2929,9 @@
       <c r="N18" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>1</v>
       </c>
@@ -2951,8 +2973,9 @@
       <c r="N19" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>1</v>
       </c>
@@ -2985,7 +3008,7 @@
         <v>28</v>
       </c>
       <c r="K20" s="10"/>
-      <c r="L20" s="21" t="s">
+      <c r="L20" s="20" t="s">
         <v>150</v>
       </c>
       <c r="M20" s="10" t="s">
@@ -2994,8 +3017,9 @@
       <c r="N20" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>1</v>
       </c>
@@ -3037,8 +3061,9 @@
       <c r="N21" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.35">
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>1</v>
       </c>
@@ -3080,7 +3105,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>1</v>
       </c>
@@ -3122,8 +3147,9 @@
       <c r="N23" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>1</v>
       </c>
@@ -3165,8 +3191,9 @@
       <c r="N24" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O24"/>
+    </row>
+    <row r="25" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>1</v>
       </c>
@@ -3208,8 +3235,9 @@
       <c r="N25" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O25"/>
+    </row>
+    <row r="26" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -3251,8 +3279,9 @@
       <c r="N26" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O26"/>
+    </row>
+    <row r="27" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>1</v>
       </c>
@@ -3294,8 +3323,9 @@
       <c r="N27" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O27"/>
+    </row>
+    <row r="28" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>1</v>
       </c>
@@ -3337,8 +3367,9 @@
       <c r="N28" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O28"/>
+    </row>
+    <row r="29" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>1</v>
       </c>
@@ -3380,8 +3411,9 @@
       <c r="N29" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O29"/>
+    </row>
+    <row r="30" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>1</v>
       </c>
@@ -3423,8 +3455,9 @@
       <c r="N30" s="10" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <v>1</v>
       </c>
@@ -3466,8 +3499,9 @@
       <c r="N31" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O31"/>
+    </row>
+    <row r="32" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>1</v>
       </c>
@@ -3509,8 +3543,9 @@
       <c r="N32" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O32"/>
+    </row>
+    <row r="33" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
         <v>1</v>
       </c>
@@ -3552,8 +3587,9 @@
       <c r="N33" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O33"/>
+    </row>
+    <row r="34" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
         <v>1</v>
       </c>
@@ -3595,8 +3631,9 @@
       <c r="N34" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O34"/>
+    </row>
+    <row r="35" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
         <v>1</v>
       </c>
@@ -3638,8 +3675,9 @@
       <c r="N35" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O35"/>
+    </row>
+    <row r="36" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
         <v>1</v>
       </c>
@@ -3681,8 +3719,9 @@
       <c r="N36" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.35">
+      <c r="O36"/>
+    </row>
+    <row r="37" spans="1:15" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <v>1</v>
       </c>
@@ -3724,8 +3763,9 @@
       <c r="N37" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.35">
+      <c r="O37"/>
+    </row>
+    <row r="38" spans="1:15" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.35">
       <c r="A38" s="10">
         <v>1</v>
       </c>
@@ -3767,8 +3807,9 @@
       <c r="N38" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.35">
+      <c r="O38"/>
+    </row>
+    <row r="39" spans="1:15" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>1</v>
       </c>
@@ -3810,8 +3851,9 @@
       <c r="N39" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O39"/>
+    </row>
+    <row r="40" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
         <v>1</v>
       </c>
@@ -3837,7 +3879,7 @@
       <c r="H40" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I40" s="22" t="s">
+      <c r="I40" s="21" t="s">
         <v>27</v>
       </c>
       <c r="J40" s="10" t="s">
@@ -3853,8 +3895,9 @@
       <c r="N40" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O40"/>
+    </row>
+    <row r="41" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
         <v>2</v>
       </c>
@@ -3896,8 +3939,9 @@
       <c r="N41" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O41"/>
+    </row>
+    <row r="42" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
         <v>2</v>
       </c>
@@ -3939,8 +3983,9 @@
       <c r="N42" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O42"/>
+    </row>
+    <row r="43" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
         <v>2</v>
       </c>
@@ -3982,8 +4027,9 @@
       <c r="N43" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" ht="30" x14ac:dyDescent="0.35">
+      <c r="O43"/>
+    </row>
+    <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.35">
       <c r="A44" s="7">
         <v>2</v>
       </c>
@@ -4025,7 +4071,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
         <v>2</v>
       </c>
@@ -4067,7 +4113,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A46" s="10">
         <v>2</v>
       </c>
@@ -4109,8 +4155,9 @@
       <c r="N46" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O46"/>
+    </row>
+    <row r="47" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A47" s="10">
         <v>2</v>
       </c>
@@ -4143,7 +4190,7 @@
         <v>28</v>
       </c>
       <c r="K47" s="10"/>
-      <c r="L47" s="21" t="s">
+      <c r="L47" s="20" t="s">
         <v>87</v>
       </c>
       <c r="M47" s="10" t="s">
@@ -4152,8 +4199,9 @@
       <c r="N47" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O47"/>
+    </row>
+    <row r="48" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A48" s="10">
         <v>2</v>
       </c>
@@ -4167,7 +4215,9 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E48" s="10"/>
+      <c r="E48" s="7">
+        <v>403</v>
+      </c>
       <c r="F48" s="10">
         <v>456</v>
       </c>
@@ -4184,7 +4234,7 @@
         <v>28</v>
       </c>
       <c r="K48" s="10"/>
-      <c r="L48" s="21" t="s">
+      <c r="L48" s="20" t="s">
         <v>151</v>
       </c>
       <c r="M48" s="10" t="s">
@@ -4193,8 +4243,9 @@
       <c r="N48" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O48"/>
+    </row>
+    <row r="49" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A49" s="10">
         <v>2</v>
       </c>
@@ -4208,7 +4259,9 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E49" s="10"/>
+      <c r="E49" s="7">
+        <v>403</v>
+      </c>
       <c r="F49" s="10">
         <v>451</v>
       </c>
@@ -4225,7 +4278,7 @@
         <v>28</v>
       </c>
       <c r="K49" s="10"/>
-      <c r="L49" s="23" t="s">
+      <c r="L49" s="22" t="s">
         <v>136</v>
       </c>
       <c r="M49" s="10" t="s">
@@ -4234,8 +4287,9 @@
       <c r="N49" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O49"/>
+    </row>
+    <row r="50" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A50" s="10">
         <v>2</v>
       </c>
@@ -4249,7 +4303,9 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E50" s="10"/>
+      <c r="E50" s="7">
+        <v>403</v>
+      </c>
       <c r="F50" s="10">
         <v>454</v>
       </c>
@@ -4266,7 +4322,7 @@
         <v>28</v>
       </c>
       <c r="K50" s="10"/>
-      <c r="L50" s="21" t="s">
+      <c r="L50" s="20" t="s">
         <v>92</v>
       </c>
       <c r="M50" s="10" t="s">
@@ -4275,8 +4331,9 @@
       <c r="N50" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O50"/>
+    </row>
+    <row r="51" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A51" s="10">
         <v>2</v>
       </c>
@@ -4290,7 +4347,9 @@
         <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
-      <c r="E51" s="10"/>
+      <c r="E51" s="7">
+        <v>505</v>
+      </c>
       <c r="F51" s="10">
         <v>452</v>
       </c>
@@ -4316,8 +4375,9 @@
       <c r="N51" s="10">
         <v>911</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O51"/>
+    </row>
+    <row r="52" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A52" s="10">
         <v>2</v>
       </c>
@@ -4331,7 +4391,9 @@
         <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
-      <c r="E52" s="10"/>
+      <c r="E52" s="7">
+        <v>501</v>
+      </c>
       <c r="F52" s="10">
         <v>456</v>
       </c>
@@ -4357,8 +4419,9 @@
       <c r="N52" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O52"/>
+    </row>
+    <row r="53" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A53" s="10">
         <v>2</v>
       </c>
@@ -4372,7 +4435,9 @@
         <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
-      <c r="E53" s="10"/>
+      <c r="E53" s="7">
+        <v>503</v>
+      </c>
       <c r="F53" s="10">
         <v>451</v>
       </c>
@@ -4398,8 +4463,9 @@
       <c r="N53" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O53"/>
+    </row>
+    <row r="54" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A54" s="10">
         <v>2</v>
       </c>
@@ -4413,7 +4479,9 @@
         <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
-      <c r="E54" s="10"/>
+      <c r="E54" s="7">
+        <v>501</v>
+      </c>
       <c r="F54" s="10">
         <v>455</v>
       </c>
@@ -4439,8 +4507,9 @@
       <c r="N54" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O54"/>
+    </row>
+    <row r="55" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A55" s="10">
         <v>2</v>
       </c>
@@ -4454,7 +4523,9 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E55" s="10"/>
+      <c r="E55" s="7">
+        <v>502</v>
+      </c>
       <c r="F55" s="10">
         <v>552</v>
       </c>
@@ -4471,7 +4542,7 @@
         <v>47</v>
       </c>
       <c r="K55" s="10"/>
-      <c r="L55" s="21" t="s">
+      <c r="L55" s="20" t="s">
         <v>152</v>
       </c>
       <c r="M55" s="10" t="s">
@@ -4480,8 +4551,9 @@
       <c r="N55" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O55"/>
+    </row>
+    <row r="56" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A56" s="10">
         <v>2</v>
       </c>
@@ -4495,7 +4567,9 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E56" s="10"/>
+      <c r="E56" s="7">
+        <v>505</v>
+      </c>
       <c r="F56" s="10">
         <v>551</v>
       </c>
@@ -4521,8 +4595,9 @@
       <c r="N56" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O56"/>
+    </row>
+    <row r="57" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A57" s="10">
         <v>2</v>
       </c>
@@ -4536,7 +4611,9 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E57" s="10"/>
+      <c r="E57" s="7">
+        <v>505</v>
+      </c>
       <c r="F57" s="10">
         <v>553</v>
       </c>
@@ -4546,7 +4623,7 @@
       <c r="H57" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I57" s="22" t="s">
+      <c r="I57" s="21" t="s">
         <v>27</v>
       </c>
       <c r="J57" s="10" t="s">
@@ -4562,8 +4639,9 @@
       <c r="N57" s="10" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O57"/>
+    </row>
+    <row r="58" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A58" s="10">
         <v>2</v>
       </c>
@@ -4577,7 +4655,9 @@
         <f t="shared" si="1"/>
         <v>-4.5</v>
       </c>
-      <c r="E58" s="10"/>
+      <c r="E58" s="7">
+        <v>603</v>
+      </c>
       <c r="F58" s="10">
         <v>156</v>
       </c>
@@ -4603,8 +4683,9 @@
       <c r="N58" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O58"/>
+    </row>
+    <row r="59" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A59" s="10">
         <v>2</v>
       </c>
@@ -4618,7 +4699,9 @@
         <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
-      <c r="E59" s="10"/>
+      <c r="E59" s="7">
+        <v>603</v>
+      </c>
       <c r="F59" s="10">
         <v>553</v>
       </c>
@@ -4644,8 +4727,9 @@
       <c r="N59" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O59"/>
+    </row>
+    <row r="60" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A60" s="10">
         <v>2</v>
       </c>
@@ -4659,7 +4743,9 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E60" s="10"/>
+      <c r="E60" s="7">
+        <v>602</v>
+      </c>
       <c r="F60" s="10">
         <v>651</v>
       </c>
@@ -4685,8 +4771,9 @@
       <c r="N60" s="10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O60"/>
+    </row>
+    <row r="61" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A61" s="10">
         <v>2</v>
       </c>
@@ -4700,7 +4787,9 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E61" s="10"/>
+      <c r="E61" s="7">
+        <v>601</v>
+      </c>
       <c r="F61" s="10">
         <v>652</v>
       </c>
@@ -4726,8 +4815,9 @@
       <c r="N61" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O61"/>
+    </row>
+    <row r="62" spans="1:15" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="10">
         <v>2</v>
       </c>
@@ -4741,7 +4831,7 @@
         <f t="shared" si="1"/>
         <v>-4.5</v>
       </c>
-      <c r="E62" s="10">
+      <c r="E62" s="7">
         <v>704</v>
       </c>
       <c r="F62" s="10">
@@ -4769,8 +4859,9 @@
       <c r="N62" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O62"/>
+    </row>
+    <row r="63" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A63" s="10">
         <v>2</v>
       </c>
@@ -4784,7 +4875,7 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="E63" s="10">
+      <c r="E63" s="7">
         <v>704</v>
       </c>
       <c r="F63" s="10">
@@ -4812,8 +4903,9 @@
       <c r="N63" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O63"/>
+    </row>
+    <row r="64" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A64" s="10">
         <v>2</v>
       </c>
@@ -4824,10 +4916,10 @@
         <v>6.5</v>
       </c>
       <c r="D64" s="10">
-        <f t="shared" ref="D64:D90" si="2">C64-B64</f>
+        <f t="shared" ref="D64:D95" si="2">C64-B64</f>
         <v>-0.5</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E64" s="7">
         <v>703</v>
       </c>
       <c r="F64" s="10">
@@ -4839,7 +4931,7 @@
       <c r="H64" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I64" s="22" t="s">
+      <c r="I64" s="21" t="s">
         <v>27</v>
       </c>
       <c r="J64" s="10" t="s">
@@ -4855,8 +4947,9 @@
       <c r="N64" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O64"/>
+    </row>
+    <row r="65" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A65" s="10">
         <v>2</v>
       </c>
@@ -4870,7 +4963,7 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
-      <c r="E65" s="10">
+      <c r="E65" s="7">
         <v>703</v>
       </c>
       <c r="F65" s="10">
@@ -4898,8 +4991,9 @@
       <c r="N65" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O65"/>
+    </row>
+    <row r="66" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A66" s="10">
         <v>2</v>
       </c>
@@ -4913,7 +5007,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E66" s="10">
+      <c r="E66" s="7">
         <v>703</v>
       </c>
       <c r="F66" s="10">
@@ -4925,7 +5019,7 @@
       <c r="H66" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I66" s="22" t="s">
+      <c r="I66" s="21" t="s">
         <v>37</v>
       </c>
       <c r="J66" s="10" t="s">
@@ -4941,8 +5035,9 @@
       <c r="N66" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O66"/>
+    </row>
+    <row r="67" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A67" s="10">
         <v>2</v>
       </c>
@@ -4956,7 +5051,7 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E67" s="10">
+      <c r="E67" s="7">
         <v>703</v>
       </c>
       <c r="F67" s="10">
@@ -4986,8 +5081,9 @@
       <c r="N67" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O67"/>
+    </row>
+    <row r="68" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A68" s="10">
         <v>2</v>
       </c>
@@ -5001,7 +5097,9 @@
         <f t="shared" si="2"/>
         <v>-3.5</v>
       </c>
-      <c r="E68" s="10"/>
+      <c r="E68" s="7">
+        <v>802</v>
+      </c>
       <c r="F68" s="10">
         <v>452</v>
       </c>
@@ -5027,8 +5125,9 @@
       <c r="N68" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O68"/>
+    </row>
+    <row r="69" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A69" s="10">
         <v>2</v>
       </c>
@@ -5042,7 +5141,9 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
-      <c r="E69" s="10"/>
+      <c r="E69" s="7">
+        <v>802</v>
+      </c>
       <c r="F69" s="10">
         <v>751</v>
       </c>
@@ -5068,8 +5169,9 @@
       <c r="N69" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O69"/>
+    </row>
+    <row r="70" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A70" s="10">
         <v>2</v>
       </c>
@@ -5083,7 +5185,9 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
-      <c r="E70" s="10"/>
+      <c r="E70" s="7">
+        <v>801</v>
+      </c>
       <c r="F70" s="10">
         <v>752</v>
       </c>
@@ -5109,8 +5213,9 @@
       <c r="N70" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O70"/>
+    </row>
+    <row r="71" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A71" s="10">
         <v>2</v>
       </c>
@@ -5124,7 +5229,9 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
-      <c r="E71" s="10"/>
+      <c r="E71" s="7">
+        <v>803</v>
+      </c>
       <c r="F71" s="10">
         <v>753</v>
       </c>
@@ -5141,7 +5248,7 @@
         <v>28</v>
       </c>
       <c r="K71" s="10"/>
-      <c r="L71" s="21" t="s">
+      <c r="L71" s="20" t="s">
         <v>153</v>
       </c>
       <c r="M71" s="10" t="s">
@@ -5150,8 +5257,9 @@
       <c r="N71" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O71"/>
+    </row>
+    <row r="72" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A72" s="10">
         <v>2</v>
       </c>
@@ -5165,7 +5273,7 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E72" s="10">
+      <c r="E72" s="7">
         <v>801</v>
       </c>
       <c r="F72" s="10">
@@ -5184,7 +5292,7 @@
         <v>28</v>
       </c>
       <c r="K72" s="10"/>
-      <c r="L72" s="21" t="s">
+      <c r="L72" s="20" t="s">
         <v>154</v>
       </c>
       <c r="M72" s="10" t="s">
@@ -5193,8 +5301,9 @@
       <c r="N72" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O72"/>
+    </row>
+    <row r="73" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A73" s="10">
         <v>2</v>
       </c>
@@ -5208,7 +5317,7 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="E73" s="10">
+      <c r="E73" s="7">
         <v>903</v>
       </c>
       <c r="F73" s="10">
@@ -5236,8 +5345,9 @@
       <c r="N73" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O73"/>
+    </row>
+    <row r="74" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="7">
         <v>2</v>
       </c>
@@ -5251,6 +5361,9 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
+      <c r="E74" s="7">
+        <v>902</v>
+      </c>
       <c r="F74" s="7">
         <v>851</v>
       </c>
@@ -5276,7 +5389,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="10">
         <v>2</v>
       </c>
@@ -5290,7 +5403,9 @@
         <f t="shared" si="2"/>
         <v>-5.5</v>
       </c>
-      <c r="E75" s="10"/>
+      <c r="E75" s="7">
+        <v>1004</v>
+      </c>
       <c r="F75" s="10">
         <v>452</v>
       </c>
@@ -5316,8 +5431,9 @@
       <c r="N75" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O75"/>
+    </row>
+    <row r="76" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A76" s="10">
         <v>2</v>
       </c>
@@ -5331,7 +5447,9 @@
         <f t="shared" si="2"/>
         <v>-3.5</v>
       </c>
-      <c r="E76" s="10"/>
+      <c r="E76" s="7">
+        <v>1004</v>
+      </c>
       <c r="F76" s="10">
         <v>654</v>
       </c>
@@ -5357,8 +5475,9 @@
       <c r="N76" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O76"/>
+    </row>
+    <row r="77" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A77" s="10">
         <v>2</v>
       </c>
@@ -5372,7 +5491,9 @@
         <f t="shared" si="2"/>
         <v>-3.5</v>
       </c>
-      <c r="E77" s="10"/>
+      <c r="E77" s="7">
+        <v>1004</v>
+      </c>
       <c r="F77" s="10">
         <v>653</v>
       </c>
@@ -5398,8 +5519,9 @@
       <c r="N77" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O77"/>
+    </row>
+    <row r="78" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A78" s="10">
         <v>2</v>
       </c>
@@ -5413,7 +5535,9 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
-      <c r="E78" s="10"/>
+      <c r="E78" s="7">
+        <v>1005</v>
+      </c>
       <c r="F78" s="10">
         <v>951</v>
       </c>
@@ -5439,8 +5563,9 @@
       <c r="N78" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O78"/>
+    </row>
+    <row r="79" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A79" s="10">
         <v>2</v>
       </c>
@@ -5454,7 +5579,9 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
-      <c r="E79" s="10"/>
+      <c r="E79" s="7">
+        <v>1002</v>
+      </c>
       <c r="F79" s="10">
         <v>952</v>
       </c>
@@ -5480,8 +5607,9 @@
       <c r="N79" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="O79"/>
+    </row>
+    <row r="80" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A80" s="10">
         <v>2</v>
       </c>
@@ -5495,7 +5623,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E80" s="10">
+      <c r="E80" s="7">
         <v>1031</v>
       </c>
       <c r="F80" s="10">
@@ -5523,6 +5651,7 @@
       <c r="N80" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="O80"/>
     </row>
     <row r="81" spans="1:46" ht="30" x14ac:dyDescent="0.35">
       <c r="A81" s="7">
@@ -5538,6 +5667,9 @@
         <f t="shared" si="2"/>
         <v>-10.5</v>
       </c>
+      <c r="E81" s="7">
+        <v>1103</v>
+      </c>
       <c r="F81" s="7">
         <v>53</v>
       </c>
@@ -5577,6 +5709,9 @@
         <f t="shared" si="2"/>
         <v>-10.5</v>
       </c>
+      <c r="E82" s="7">
+        <v>1103</v>
+      </c>
       <c r="F82" s="7">
         <v>55</v>
       </c>
@@ -5829,6 +5964,9 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
+      <c r="E88" s="7">
+        <v>1102</v>
+      </c>
       <c r="F88" s="7">
         <v>1053</v>
       </c>
@@ -5868,6 +6006,9 @@
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
+      <c r="E89" s="7">
+        <v>1102</v>
+      </c>
       <c r="F89" s="7">
         <v>1052</v>
       </c>
@@ -5934,7 +6075,6 @@
       <c r="N90" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="O90"/>
       <c r="P90"/>
       <c r="Q90"/>
       <c r="R90"/>
@@ -5967,8 +6107,240 @@
       <c r="AS90"/>
       <c r="AT90"/>
     </row>
-    <row r="93" spans="1:46" ht="31" x14ac:dyDescent="0.35">
-      <c r="G93" s="20"/>
+    <row r="91" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A91" s="7">
+        <v>1</v>
+      </c>
+      <c r="B91" s="7">
+        <v>3</v>
+      </c>
+      <c r="C91" s="7">
+        <v>2</v>
+      </c>
+      <c r="D91" s="7">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E91" s="7">
+        <v>303</v>
+      </c>
+      <c r="F91" s="7">
+        <v>233</v>
+      </c>
+      <c r="G91" s="7">
+        <v>1</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J91" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L91" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M91" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N91" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O91">
+        <v>1</v>
+      </c>
+      <c r="AS91"/>
+      <c r="AT91"/>
+    </row>
+    <row r="92" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A92" s="7">
+        <v>1</v>
+      </c>
+      <c r="B92" s="7">
+        <v>9</v>
+      </c>
+      <c r="C92" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="D92" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="E92" s="7">
+        <v>901</v>
+      </c>
+      <c r="F92" s="7">
+        <v>881</v>
+      </c>
+      <c r="G92" s="7">
+        <v>1</v>
+      </c>
+      <c r="H92" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I92" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J92" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L92" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M92" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N92" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O92">
+        <v>1</v>
+      </c>
+      <c r="AS92"/>
+      <c r="AT92"/>
+    </row>
+    <row r="93" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A93" s="7">
+        <v>1</v>
+      </c>
+      <c r="B93" s="7">
+        <v>9</v>
+      </c>
+      <c r="C93" s="7">
+        <v>10</v>
+      </c>
+      <c r="D93" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E93" s="7">
+        <v>904</v>
+      </c>
+      <c r="F93" s="7">
+        <v>1031</v>
+      </c>
+      <c r="G93" s="7">
+        <v>1</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I93" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J93" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L93" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M93" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N93" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O93">
+        <v>1</v>
+      </c>
+      <c r="AS93"/>
+      <c r="AT93"/>
+    </row>
+    <row r="94" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A94" s="7">
+        <v>1</v>
+      </c>
+      <c r="B94" s="7">
+        <v>11</v>
+      </c>
+      <c r="C94" s="7">
+        <v>10</v>
+      </c>
+      <c r="D94" s="7">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E94" s="7">
+        <v>1106</v>
+      </c>
+      <c r="F94" s="7">
+        <v>1031</v>
+      </c>
+      <c r="G94" s="7">
+        <v>1</v>
+      </c>
+      <c r="H94" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I94" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J94" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L94" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M94" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N94" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O94">
+        <v>1</v>
+      </c>
+      <c r="AS94"/>
+      <c r="AT94"/>
+    </row>
+    <row r="95" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A95" s="7">
+        <v>1</v>
+      </c>
+      <c r="B95" s="7">
+        <v>11</v>
+      </c>
+      <c r="C95" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="D95" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="E95" s="7">
+        <v>1105</v>
+      </c>
+      <c r="F95" s="7">
+        <v>1081</v>
+      </c>
+      <c r="G95" s="7">
+        <v>1</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J95" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L95" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="M95" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="N95" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O95">
+        <v>1</v>
+      </c>
+      <c r="AS95"/>
+      <c r="AT95"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N90">

</xml_diff>